<commit_message>
icdc suite for testing breed single filter
</commit_message>
<xml_diff>
--- a/InputFiles/ICDC_CaseDetails.xlsx
+++ b/InputFiles/ICDC_CaseDetails.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\radhakrishnang2\Desktop\March\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFBBDFA-46E8-485A-A6C4-E1ACE1148AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DF74F90-3D26-43E7-B901-2F946EB63137}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DemographicsSingle" sheetId="2" r:id="rId1"/>
@@ -25,31 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>breed</t>
-  </si>
-  <si>
-    <t>sex</t>
-  </si>
-  <si>
-    <t>neutStatus</t>
-  </si>
-  <si>
-    <t>weight</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>Basset Hound</t>
-  </si>
-  <si>
-    <t>Male</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="90">
   <si>
     <t>case/UBC01-781-811-Vm13</t>
   </si>
@@ -70,12 +46,6 @@
   </si>
   <si>
     <t>statQuery</t>
-  </si>
-  <si>
-    <t>TC01_Canine_CaseDetail_UBC01_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_Canine_CaseDetail_UBC01_WebData.xlsx</t>
   </si>
   <si>
     <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
@@ -147,6 +117,898 @@
 order by samp.sample_id , f.file_type asc
 limit 25</t>
   </si>
+  <si>
+    <t>demographicsQuery</t>
+  </si>
+  <si>
+    <t>diagnosisQuery</t>
+  </si>
+  <si>
+    <t>studyQuery</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['UBC01-781-811-Vm13']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+        coalesce(demo.breed, '') AS BREED ,
+      coalesce(demo.sex, '') AS SEX,
+       coalesce(demo.neutered_indicator, '') AS `NEUTERED STATUS`,
+        coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `WEIGHT`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS `AGE AT ENROLLMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['UBC01-781-811-Vm13']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN         
+ coalesce(diag.disease_term, '') AS DISEASE ,
+        coalesce(diag.stage_of_disease, '') AS `STAGE OF DISEASE` ,
+coalesce(diag.date_of_diagnosis,'') as `DATE OF DIAGNOSIS`,
+coalesce(diag.primary_disease_site,'') as `PRIMARY DISEASE SITE`,
+coalesce(diag.histology_cytopathology,'') as `HISTOLOGY/CYTOLOGY`,
+coalesce(diag.histological_grade, '') as `HISTOLOGICAL GRADE`,
+   coalesce(diag.best_response, '') AS `RESPONSE TO TREATMENT`</t>
+  </si>
+  <si>
+    <t>GLIOMA01-i_0DC4</t>
+  </si>
+  <si>
+    <t>case/GLIOMA01-i_0DC4</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['GLIOMA01-i_0DC4']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+        coalesce(demo.breed, '') AS BREED ,
+      coalesce(demo.sex, '') AS SEX,
+       coalesce(demo.neutered_indicator, '') AS `NEUTERED STATUS`,
+        coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `WEIGHT`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS `AGE AT ENROLLMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['GLIOMA01-i_0DC4']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN         
+ coalesce(diag.disease_term, '') AS DISEASE ,
+        coalesce(diag.stage_of_disease, '') AS `STAGE OF DISEASE` ,
+coalesce(diag.date_of_diagnosis,'') as `DATE OF DIAGNOSIS`,
+coalesce(diag.primary_disease_site,'') as `PRIMARY DISEASE SITE`,
+coalesce(diag.histology_cytopathology,'') as `HISTOLOGY/CYTOLOGY`,
+coalesce(diag.histological_grade, '') as `HISTOLOGICAL GRADE`,
+   coalesce(diag.best_response, '') AS `RESPONSE TO TREATMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE c.case_id IN ['GLIOMA01-i_0DC4'] 
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['GLIOMA01-i_0DC4'] 
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`
+order by samp.sample_id , f.file_type asc
+limit 25</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE c.case_id IN ['GLIOMA01-i_0DC4'] 
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>TC_GLIOMA01-i_0DC4_Canine_CaseDetail_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC_GLIOMA01-i_0DC4_Canine_CaseDetail_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>TC_UBC01-781-811-Vm13_Canine_CaseDetail_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC_UBC01-781-811-Vm13_Canine_CaseDetail_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>case/MGT01-401188</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['MGT01-401188']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+        coalesce(demo.breed, '') AS BREED ,
+      coalesce(demo.sex, '') AS SEX,
+       coalesce(demo.neutered_indicator, '') AS `NEUTERED STATUS`,
+        coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `WEIGHT`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS `AGE AT ENROLLMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['MGT01-401188']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN         
+ coalesce(diag.disease_term, '') AS DISEASE ,
+        coalesce(diag.stage_of_disease, '') AS `STAGE OF DISEASE` ,
+coalesce(diag.date_of_diagnosis,'') as `DATE OF DIAGNOSIS`,
+coalesce(diag.primary_disease_site,'') as `PRIMARY DISEASE SITE`,
+coalesce(diag.histology_cytopathology,'') as `HISTOLOGY/CYTOLOGY`,
+coalesce(diag.histological_grade, '') as `HISTOLOGICAL GRADE`,
+   coalesce(diag.best_response, '') AS `RESPONSE TO TREATMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE c.case_id IN ['MGT01-401188'] 
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['MGT01-401188'] 
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`
+order by samp.sample_id , f.file_type asc
+limit 25</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE c.case_id IN ['MGT01-401188'] 
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>TC_MGT01-401188_Canine_CaseDetail_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC_MGT01-401188_Canine_CaseDetail_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MGT01-401188</t>
+  </si>
+  <si>
+    <t>case/NCATS-COP01-CCB010208</t>
+  </si>
+  <si>
+    <t>NCATS-COP01-CCB010208</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['NCATS-COP01-CCB010208']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN         
+ coalesce(diag.disease_term, '') AS DISEASE ,
+        coalesce(diag.stage_of_disease, '') AS `STAGE OF DISEASE` ,
+coalesce(diag.date_of_diagnosis,'') as `DATE OF DIAGNOSIS`,
+coalesce(diag.primary_disease_site,'') as `PRIMARY DISEASE SITE`,
+coalesce(diag.histology_cytopathology,'') as `HISTOLOGY/CYTOLOGY`,
+coalesce(diag.histological_grade, '') as `HISTOLOGICAL GRADE`,
+   coalesce(diag.best_response, '') AS `RESPONSE TO TREATMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['NCATS-COP01-CCB010208']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+        coalesce(demo.breed, '') AS BREED ,
+      coalesce(demo.sex, '') AS SEX,
+       coalesce(demo.neutered_indicator, '') AS `NEUTERED STATUS`,
+        coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `WEIGHT`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS `AGE AT ENROLLMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE c.case_id IN ['NCATS-COP01-CCB010208'] 
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['NCATS-COP01-CCB010208'] 
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`
+order by samp.sample_id , f.file_type asc
+limit 25</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE c.case_id IN ['NCATS-COP01-CCB010208'] 
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>TC_NCATS-COP01-CCB010208_Canine_CaseDetail_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC_NCATS-COP01-CCB010208_Canine_CaseDetail_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>OSA01-E4</t>
+  </si>
+  <si>
+    <t>case/OSA01-E4</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['OSA01-E4']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+        coalesce(demo.breed, '') AS BREED ,
+      coalesce(demo.sex, '') AS SEX,
+       coalesce(demo.neutered_indicator, '') AS `NEUTERED STATUS`,
+        coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `WEIGHT`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS `AGE AT ENROLLMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['OSA01-E4']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN         
+ coalesce(diag.disease_term, '') AS DISEASE ,
+        coalesce(diag.stage_of_disease, '') AS `STAGE OF DISEASE` ,
+coalesce(diag.date_of_diagnosis,'') as `DATE OF DIAGNOSIS`,
+coalesce(diag.primary_disease_site,'') as `PRIMARY DISEASE SITE`,
+coalesce(diag.histology_cytopathology,'') as `HISTOLOGY/CYTOLOGY`,
+coalesce(diag.histological_grade, '') as `HISTOLOGICAL GRADE`,
+   coalesce(diag.best_response, '') AS `RESPONSE TO TREATMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE c.case_id IN ['OSA01-E4'] 
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['OSA01-E4'] 
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`
+order by samp.sample_id , f.file_type asc
+limit 25</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE c.case_id IN ['OSA01-E4'] 
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>TC_OSA01-E4_Canine_CaseDetail_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC_OSA01-E4_Canine_CaseDetail_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>case/TCL01-BRMCT</t>
+  </si>
+  <si>
+    <t>TCL01-BRMCT</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['TCL01-BRMCT']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+        coalesce(demo.breed, '') AS BREED ,
+      coalesce(demo.sex, '') AS SEX,
+       coalesce(demo.neutered_indicator, '') AS `NEUTERED STATUS`,
+        coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `WEIGHT`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS `AGE AT ENROLLMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['TCL01-BRMCT']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN         
+ coalesce(diag.disease_term, '') AS DISEASE ,
+        coalesce(diag.stage_of_disease, '') AS `STAGE OF DISEASE` ,
+coalesce(diag.date_of_diagnosis,'') as `DATE OF DIAGNOSIS`,
+coalesce(diag.primary_disease_site,'') as `PRIMARY DISEASE SITE`,
+coalesce(diag.histology_cytopathology,'') as `HISTOLOGY/CYTOLOGY`,
+coalesce(diag.histological_grade, '') as `HISTOLOGICAL GRADE`,
+   coalesce(diag.best_response, '') AS `RESPONSE TO TREATMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE c.case_id IN ['TCL01-BRMCT'] 
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['TCL01-BRMCT'] 
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`
+order by samp.sample_id , f.file_type asc
+limit 25</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE c.case_id IN ['TCL01-BRMCT'] 
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>TC_TCL01-BRMCT_Canine_CaseDetail_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC_TCL01-BRMCT_Canine_CaseDetail_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>TCL01-CLL-1390</t>
+  </si>
+  <si>
+    <t>case/TCL01-CLL-1390</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['TCL01-CLL-1390']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+        coalesce(demo.breed, '') AS BREED ,
+      coalesce(demo.sex, '') AS SEX,
+       coalesce(demo.neutered_indicator, '') AS `NEUTERED STATUS`,
+        coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `WEIGHT`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS `AGE AT ENROLLMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['TCL01-CLL-1390']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN         
+ coalesce(diag.disease_term, '') AS DISEASE ,
+        coalesce(diag.stage_of_disease, '') AS `STAGE OF DISEASE` ,
+coalesce(diag.date_of_diagnosis,'') as `DATE OF DIAGNOSIS`,
+coalesce(diag.primary_disease_site,'') as `PRIMARY DISEASE SITE`,
+coalesce(diag.histology_cytopathology,'') as `HISTOLOGY/CYTOLOGY`,
+coalesce(diag.histological_grade, '') as `HISTOLOGICAL GRADE`,
+   coalesce(diag.best_response, '') AS `RESPONSE TO TREATMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE c.case_id IN ['TCL01-CLL-1390'] 
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['TCL01-CLL-1390'] 
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`
+order by samp.sample_id , f.file_type asc
+limit 25</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE c.case_id IN ['TCL01-CLL-1390'] 
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>TC_TCL01-CLL-1390_Canine_CaseDetail_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC_TCL01-CLL-1390_Canine_CaseDetail_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>UBC02-731-763-Mis</t>
+  </si>
+  <si>
+    <t>case/UBC02-731-763-Mis</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['UBC02-731-763-Mis']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN  
+        coalesce(demo.breed, '') AS BREED ,
+      coalesce(demo.sex, '') AS SEX,
+       coalesce(demo.neutered_indicator, '') AS `NEUTERED STATUS`,
+        coalesce(CASE weight % 1 WHEN 0 THEN apoc.convert.toInteger(weight) ELSE weight END, '') AS `WEIGHT`,
+       CASE age % 1 WHEN 0 THEN apoc.convert.toInteger(age) ELSE age END AS `AGE AT ENROLLMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['UBC02-731-763-Mis']
+MATCH (c)&lt;--(diag:diagnosis)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (co:cohort)&lt;-[*]-(c)
+WITH DISTINCT c, s, demo, diag, co, demo.patient_age_at_enrollment AS age, demo.weight as weight
+RETURN         
+ coalesce(diag.disease_term, '') AS DISEASE ,
+        coalesce(diag.stage_of_disease, '') AS `STAGE OF DISEASE` ,
+coalesce(diag.date_of_diagnosis,'') as `DATE OF DIAGNOSIS`,
+coalesce(diag.primary_disease_site,'') as `PRIMARY DISEASE SITE`,
+coalesce(diag.histology_cytopathology,'') as `HISTOLOGY/CYTOLOGY`,
+coalesce(diag.histological_grade, '') as `HISTOLOGICAL GRADE`,
+   coalesce(diag.best_response, '') AS `RESPONSE TO TREATMENT`</t>
+  </si>
+  <si>
+    <t>MATCH (s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic), (samp:sample)--&gt;(c)&lt;--(diag:diagnosis) 
+WHERE c.case_id IN ['UBC02-731-763-Mis'] 
+WITH DISTINCT samp AS samp, c, demo, diag
+RETURN  coalesce(samp.sample_id, '') AS `Sample ID`, 
+        coalesce(samp.sample_site, '') AS `Sample Site`,
+        coalesce(samp.summarized_sample_type, '') AS `Sample Type`,
+        coalesce(samp.specific_sample_pathology, '') AS `Pathology/Morphology`,
+        coalesce(samp.tumor_grade, '') AS `Tumor Grade`,
+        coalesce(samp.sample_chronology, '') AS `Sample Chronology`,
+        coalesce(samp.percentage_tumor, '') AS `Percentage Tumor`,
+        coalesce(samp.necropsy_sample, '') AS `Necropsy Sample`,
+        coalesce(samp.sample_preservation, '') AS `Sample Preservation`
+order by samp.sample_id asc
+limit 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)--&gt;(parent)
+WITH DISTINCT f, parent
+MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f)-[*]-&gt;(samp:sample)
+MATCH (f)-[*]-&gt;(c:case)&lt;--(demo:demographic)
+WHERE c.case_id IN ['UBC02-731-763-Mis'] 
+OPTIONAL MATCH (s:study)&lt;--(c)&lt;--(diag:diagnosis)&lt;-[*]-(samp)
+WITH
+        f, parent, c, demo, diag, s, samp,
+        ['Bytes', 'KB', 'MB', 'GB', 'TB'] AS units,
+        toInteger(floor(log(f.file_size)/log(1024))) as i,
+        2 as precision
+WITH
+        f, parent, c, demo, diag, s, samp,
+        f.file_size /(1024^i) AS value, 
+        10^precision AS factor,
+        units[i] as unit
+WITH    
+        f, parent, c, demo, diag, s, samp, unit,
+        round(factor * value)/factor AS size
+RETURN 
+        coalesce(samp.sample_id, '') AS `Sample ID`,
+        coalesce(f.file_name, '') AS `File Name`,
+        coalesce(f.file_type, '') AS `File Type`,
+        coalesce(f.file_format, '') AS `Format`,
+        CASE size % 1 WHEN 0 THEN apoc.convert.toInteger(size)+' ' +unit ELSE size+' ' +unit END AS Size,
+        coalesce(labels(parent)[0], '') AS `Association`,
+        coalesce(f.file_description, '') AS `Description`
+order by samp.sample_id , f.file_type asc
+limit 25</t>
+  </si>
+  <si>
+    <t>MATCH (p:program)&lt;--(s:study)&lt;-[*]-(c:case)&lt;--(demo:demographic)
+OPTIONAL MATCH (samp:sample)--&gt;(c)
+OPTIONAL MATCH (diag:diagnosis)--&gt;(c)
+OPTIONAL MATCH (f:file)-[*]-&gt;(c)
+OPTIONAL MATCH (sf:file)--&gt;(s)
+WITH DISTINCT f, sf, samp AS samp, c, demo, diag, s, p
+WHERE c.case_id IN ['UBC02-731-763-Mis'] 
+RETURN  
+    count(distinct p) AS Programs,
+    count(distinct s) AS Studies,
+    count(distinct c) AS Cases,
+    count(distinct samp) AS Samples,
+    count(distinct f) AS `Case Files`,
+    count(distinct sf) AS `Study Files`</t>
+  </si>
+  <si>
+    <t>TC_UBC02-731-763-Mis_Canine_CaseDetail_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC_UBC02-731-763-Mis_Canine_CaseDetail_WebData.xlsx</t>
+  </si>
+  <si>
+    <t>MATCH (c:case{case_id: "UBC01-781-811-Vm13"})
+OPTIONAL MATCH (c)--&gt;(co:cohort)
+OPTIONAL MATCH (c)--&gt;(s:study)
+OPTIONAL MATCH (c)&lt;--(e:enrollment)
+RETURN 
+	coalesce(s.clinical_study_designation,'') AS `ASSIGNED TO STUDY`,
+	coalesce(co.study_arm,'') AS `ASSIGNED TO ARM`,
+	coalesce(co.cohort_description,'') AS `ASSIGNED TO COHORT`,
+	coalesce(e.patient_subgroup,'') AS `PATIENT SUBGROUP`,
+	coalesce(e.date_of_informed_consent,'') AS `DATE OF INFORMED CONSENT`,
+	coalesce(e.date_of_registration, '') AS `DATE OF REGISTRATION`,
+	coalesce(e.site_short_name, '') AS `STUDY SITE`</t>
+  </si>
+  <si>
+    <t>MATCH (c:case{case_id: "GLIOMA01-i_0DC4"})
+OPTIONAL MATCH (c)--&gt;(co:cohort)
+OPTIONAL MATCH (c)--&gt;(s:study)
+OPTIONAL MATCH (c)&lt;--(e:enrollment) RETURN 
+	coalesce(s.clinical_study_designation,'') AS `ASSIGNED TO STUDY`,
+	coalesce(co.study_arm,'') AS `ASSIGNED TO ARM`,
+	coalesce(co.cohort_description,'') AS `ASSIGNED TO COHORT`,
+	coalesce(e.patient_subgroup,'') AS `PATIENT SUBGROUP`,
+	coalesce(e.date_of_informed_consent,'') AS `DATE OF INFORMED CONSENT`,
+	coalesce(e.date_of_registration, '') AS `DATE OF REGISTRATION`,
+	coalesce(e.site_short_name, '') AS `STUDY SITE`</t>
+  </si>
+  <si>
+    <t>MATCH (c:case{case_id: "MGT01-401188"})
+OPTIONAL MATCH (c)--&gt;(co:cohort)
+OPTIONAL MATCH (c)--&gt;(s:study)
+OPTIONAL MATCH (c)&lt;--(e:enrollment)  RETURN 
+	coalesce(s.clinical_study_designation,'') AS `ASSIGNED TO STUDY`,
+	coalesce(co.study_arm,'') AS `ASSIGNED TO ARM`,
+	coalesce(co.cohort_description,'') AS `ASSIGNED TO COHORT`,
+	coalesce(e.patient_subgroup,'') AS `PATIENT SUBGROUP`,
+	coalesce(e.date_of_informed_consent,'') AS `DATE OF INFORMED CONSENT`,
+	coalesce(e.date_of_registration, '') AS `DATE OF REGISTRATION`,
+	coalesce(e.site_short_name, '') AS `STUDY SITE`</t>
+  </si>
+  <si>
+    <t>MATCH (c:case{case_id: "NCATS-COP01-CCB010208"})
+OPTIONAL MATCH (c)--&gt;(co:cohort)
+OPTIONAL MATCH (c)--&gt;(s:study)
+OPTIONAL MATCH (c)&lt;--(e:enrollment) RETURN 
+	coalesce(s.clinical_study_designation,'') AS `ASSIGNED TO STUDY`,
+	coalesce(co.study_arm,'') AS `ASSIGNED TO ARM`,
+	coalesce(co.cohort_description,'') AS `ASSIGNED TO COHORT`,
+	coalesce(e.patient_subgroup,'') AS `PATIENT SUBGROUP`,
+	coalesce(e.date_of_informed_consent,'') AS `DATE OF INFORMED CONSENT`,
+	coalesce(e.date_of_registration, '') AS `DATE OF REGISTRATION`,
+	coalesce(e.site_short_name, '') AS `STUDY SITE`</t>
+  </si>
+  <si>
+    <t>MATCH (c:case{case_id: "OSA01-E4"})
+OPTIONAL MATCH (c)--&gt;(co:cohort)
+OPTIONAL MATCH (c)--&gt;(s:study)
+OPTIONAL MATCH (c)&lt;--(e:enrollment) RETURN 
+	coalesce(s.clinical_study_designation,'') AS `ASSIGNED TO STUDY`,
+	coalesce(co.study_arm,'') AS `ASSIGNED TO ARM`,
+	coalesce(co.cohort_description,'') AS `ASSIGNED TO COHORT`,
+	coalesce(e.patient_subgroup,'') AS `PATIENT SUBGROUP`,
+	coalesce(e.date_of_informed_consent,'') AS `DATE OF INFORMED CONSENT`,
+	coalesce(e.date_of_registration, '') AS `DATE OF REGISTRATION`,
+	coalesce(e.site_short_name, '') AS `STUDY SITE`</t>
+  </si>
+  <si>
+    <t>MATCH (c:case{case_id: "TCL01-BRMCT"})
+OPTIONAL MATCH (c)--&gt;(co:cohort)
+OPTIONAL MATCH (c)--&gt;(s:study)
+OPTIONAL MATCH (c)&lt;--(e:enrollment) RETURN 
+	coalesce(s.clinical_study_designation,'') AS `ASSIGNED TO STUDY`,
+	coalesce(co.study_arm,'') AS `ASSIGNED TO ARM`,
+	coalesce(co.cohort_description,'') AS `ASSIGNED TO COHORT`,
+	coalesce(e.patient_subgroup,'') AS `PATIENT SUBGROUP`,
+	coalesce(e.date_of_informed_consent,'') AS `DATE OF INFORMED CONSENT`,
+	coalesce(e.date_of_registration, '') AS `DATE OF REGISTRATION`,
+	coalesce(e.site_short_name, '') AS `STUDY SITE`</t>
+  </si>
+  <si>
+    <t>MATCH (c:case{case_id: "TCL01-CLL-1390"})
+OPTIONAL MATCH (c)--&gt;(co:cohort)
+OPTIONAL MATCH (c)--&gt;(s:study)
+OPTIONAL MATCH (c)&lt;--(e:enrollment) RETURN 
+	coalesce(s.clinical_study_designation,'') AS `ASSIGNED TO STUDY`,
+	coalesce(co.study_arm,'') AS `ASSIGNED TO ARM`,
+	coalesce(co.cohort_description,'') AS `ASSIGNED TO COHORT`,
+	coalesce(e.patient_subgroup,'') AS `PATIENT SUBGROUP`,
+	coalesce(e.date_of_informed_consent,'') AS `DATE OF INFORMED CONSENT`,
+	coalesce(e.date_of_registration, '') AS `DATE OF REGISTRATION`,
+	coalesce(e.site_short_name, '') AS `STUDY SITE`</t>
+  </si>
+  <si>
+    <t>MATCH (c:case{case_id: "UBC02-731-763-Mis"})
+OPTIONAL MATCH (c)--&gt;(co:cohort)
+OPTIONAL MATCH (c)--&gt;(s:study)
+OPTIONAL MATCH (c)&lt;--(e:enrollment) RETURN 
+	coalesce(s.clinical_study_designation,'') AS `ASSIGNED TO STUDY`,
+	coalesce(co.study_arm,'') AS `ASSIGNED TO ARM`,
+	coalesce(co.cohort_description,'') AS `ASSIGNED TO COHORT`,
+	coalesce(e.patient_subgroup,'') AS `PATIENT SUBGROUP`,
+	coalesce(e.date_of_informed_consent,'') AS `DATE OF INFORMED CONSENT`,
+	coalesce(e.date_of_registration, '') AS `DATE OF REGISTRATION`,
+	coalesce(e.site_short_name, '') AS `STUDY SITE`</t>
+  </si>
 </sst>
 </file>
 
@@ -161,12 +1023,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -181,10 +1055,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -467,98 +1347,311 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFEFD21-1923-4751-BACE-62DAB7BF55BF}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="72.42578125" customWidth="1"/>
-    <col min="9" max="9" width="74.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="63.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="45" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="38.5703125" customWidth="1"/>
+    <col min="6" max="6" width="72.42578125" customWidth="1"/>
+    <col min="7" max="7" width="74.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="45" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1">
+    <row r="4" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="1">
-        <v>11.3</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>16</v>
+      <c r="C4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>